<commit_message>
MML4 vital sign updated, working on flow sheet
</commit_message>
<xml_diff>
--- a/mapping/mml4_vital_sign.xlsx
+++ b/mapping/mml4_vital_sign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="23715" windowHeight="10050"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15240" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="246">
   <si>
     <t>Elements</t>
   </si>
@@ -283,10 +283,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0011.1]/value</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Identifier</t>
   </si>
   <si>
@@ -299,14 +295,6 @@
   </si>
   <si>
     <t>DV_TEXT</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0011.1]/mappings/target/defining_code/terminology_id/value</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0011.1]/mappings/match</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -353,17 +341,6 @@
   </si>
   <si>
     <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1]/items[openEHR-EHR-CLUSTER.person_name.v1]/items[at0001]/value</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1]/items[at0003]/items[at0011]</t>
-  </si>
-  <si>
-    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1]/items[at0003]/items[at0011]/mappings/target/defining_code/terminology_id/value</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1]/items[at0003]/items[at0011]/mappings/match</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1117,6 +1094,38 @@
   </si>
   <si>
     <t>/content[openEHR-EHR-SECTION.vital_signs.v1]/items[openEHR-EHR-OBSERVATION.lab_test.v1]/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.specimen.v1]/items[openEHR-EHR-CLUSTER.anatomical_location.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Facility']/items[at0001]/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Facility']/items[at0011]/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Facility']/items[at0011]/mappings/target/defining_code/terminology_id/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Facility']/items[at0011]/mappings/match</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Profesional Identifier</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1]/items[at0003]/items[at0013]/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1]/items[at0003]/items[at0013]/mappings/target/defining_code/terminology_id/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1]/items[at0003]/items[at0013]/mappings/match</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1664,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="H207" sqref="H207"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1710,7 +1719,7 @@
     </row>
     <row r="2" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1780,7 +1789,7 @@
         <v>57</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>61</v>
+        <v>238</v>
       </c>
       <c r="K5" s="16"/>
     </row>
@@ -1799,13 +1808,13 @@
       <c r="F6" s="14"/>
       <c r="G6" s="15"/>
       <c r="H6" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>58</v>
+        <v>239</v>
       </c>
       <c r="K6" s="16"/>
     </row>
@@ -1828,7 +1837,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15" t="s">
-        <v>63</v>
+        <v>240</v>
       </c>
       <c r="K7" s="16"/>
     </row>
@@ -1841,11 +1850,11 @@
       <c r="F8" s="14"/>
       <c r="G8" s="15"/>
       <c r="H8" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15" t="s">
-        <v>64</v>
+        <v>241</v>
       </c>
       <c r="K8" s="16"/>
     </row>
@@ -1869,10 +1878,10 @@
         <v>55</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9" s="16"/>
     </row>
@@ -1893,13 +1902,13 @@
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K10" s="16"/>
     </row>
@@ -1920,7 +1929,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K11" s="16"/>
     </row>
@@ -1933,11 +1942,11 @@
       <c r="F12" s="14"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I12" s="15"/>
       <c r="J12" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K12" s="16"/>
     </row>
@@ -1964,7 +1973,7 @@
         <v>57</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K13" s="16"/>
     </row>
@@ -1985,13 +1994,13 @@
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K14" s="16"/>
     </row>
@@ -2012,7 +2021,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K15" s="16"/>
     </row>
@@ -2025,11 +2034,11 @@
       <c r="F16" s="14"/>
       <c r="G16" s="15"/>
       <c r="H16" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I16" s="15"/>
       <c r="J16" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K16" s="16"/>
     </row>
@@ -2053,10 +2062,10 @@
         <v>54</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K17" s="16"/>
     </row>
@@ -2076,12 +2085,14 @@
         <v>24</v>
       </c>
       <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="H18" s="8" t="s">
+        <v>242</v>
+      </c>
       <c r="I18" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>75</v>
+        <v>243</v>
       </c>
       <c r="K18" s="16"/>
     </row>
@@ -2102,7 +2113,7 @@
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15" t="s">
-        <v>76</v>
+        <v>244</v>
       </c>
       <c r="K19" s="16"/>
     </row>
@@ -2115,11 +2126,11 @@
       <c r="F20" s="14"/>
       <c r="G20" s="15"/>
       <c r="H20" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I20" s="15"/>
       <c r="J20" s="15" t="s">
-        <v>77</v>
+        <v>245</v>
       </c>
       <c r="K20" s="16"/>
     </row>
@@ -2128,7 +2139,7 @@
         <v>1.5</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="25" t="s">
@@ -2140,13 +2151,13 @@
       <c r="F21" s="26"/>
       <c r="G21" s="19"/>
       <c r="H21" s="27" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K21" s="20"/>
     </row>
@@ -2164,7 +2175,7 @@
     </row>
     <row r="23" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -2212,7 +2223,7 @@
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
@@ -2256,13 +2267,13 @@
       <c r="F27" s="14"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K27" s="16"/>
     </row>
@@ -2287,7 +2298,7 @@
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="K28" s="16"/>
     </row>
@@ -2308,13 +2319,13 @@
       <c r="F29" s="14"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="K29" s="16"/>
     </row>
@@ -2334,10 +2345,10 @@
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="K30" s="16"/>
     </row>
@@ -2377,22 +2388,22 @@
       <c r="F32" s="14"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="K32" s="16"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A33" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="14" t="s">
@@ -2404,22 +2415,22 @@
       <c r="F33" s="14"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="K33" s="16"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A34" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="14" t="s">
@@ -2429,7 +2440,7 @@
         <v>7</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="8"/>
@@ -2439,10 +2450,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14" t="s">
@@ -2454,22 +2465,22 @@
       <c r="F35" s="14"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="K35" s="16"/>
     </row>
     <row r="36" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18" t="s">
@@ -2481,19 +2492,19 @@
       <c r="F36" s="18"/>
       <c r="G36" s="19"/>
       <c r="H36" s="19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="K36" s="20"/>
     </row>
     <row r="38" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.15">
@@ -2531,7 +2542,7 @@
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I40" s="15"/>
       <c r="J40" s="16"/>
@@ -2573,13 +2584,13 @@
       <c r="F42" s="14"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.15">
@@ -2603,7 +2614,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.15">
@@ -2623,13 +2634,13 @@
       <c r="F44" s="14"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.15">
@@ -2648,10 +2659,10 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.15">
@@ -2694,10 +2705,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A48" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14" t="s">
@@ -2709,21 +2720,21 @@
       <c r="F48" s="14"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="14" t="s">
@@ -2733,7 +2744,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G49" s="15"/>
       <c r="H49" s="14"/>
@@ -2742,10 +2753,10 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14" t="s">
@@ -2757,21 +2768,21 @@
       <c r="F50" s="14"/>
       <c r="G50" s="15"/>
       <c r="H50" s="15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="18" t="s">
@@ -2783,13 +2794,13 @@
       <c r="F51" s="18"/>
       <c r="G51" s="19"/>
       <c r="H51" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J51" s="20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.15">
@@ -2802,7 +2813,7 @@
     </row>
     <row r="54" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2845,7 +2856,7 @@
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="15" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I56" s="15"/>
       <c r="J56" s="16"/>
@@ -2887,13 +2898,13 @@
       <c r="F58" s="14"/>
       <c r="G58" s="15"/>
       <c r="H58" s="15" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J58" s="16" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.15">
@@ -2917,7 +2928,7 @@
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
       <c r="J59" s="16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.15">
@@ -2937,13 +2948,13 @@
       <c r="F60" s="14"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I60" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J60" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.15">
@@ -2963,7 +2974,7 @@
       </c>
       <c r="G61" s="15"/>
       <c r="H61" s="15" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I61" s="15"/>
       <c r="J61" s="16"/>
@@ -3005,13 +3016,13 @@
       <c r="F63" s="14"/>
       <c r="G63" s="15"/>
       <c r="H63" s="15" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I63" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J63" s="16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.15">
@@ -3035,7 +3046,7 @@
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
       <c r="J64" s="16" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.15">
@@ -3055,13 +3066,13 @@
       <c r="F65" s="14"/>
       <c r="G65" s="15"/>
       <c r="H65" s="15" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I65" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J65" s="16" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.15">
@@ -3080,10 +3091,10 @@
       <c r="G66" s="15"/>
       <c r="H66" s="15"/>
       <c r="I66" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J66" s="16" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.15">
@@ -3121,21 +3132,21 @@
       <c r="F68" s="14"/>
       <c r="G68" s="15"/>
       <c r="H68" s="15" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I68" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J68" s="16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A69" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C69" s="14"/>
       <c r="D69" s="14" t="s">
@@ -3147,21 +3158,21 @@
       <c r="F69" s="14"/>
       <c r="G69" s="15"/>
       <c r="H69" s="15" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J69" s="16" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A70" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C70" s="14"/>
       <c r="D70" s="14" t="s">
@@ -3171,25 +3182,25 @@
         <v>7</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J70" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A71" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C71" s="14"/>
       <c r="D71" s="14" t="s">
@@ -3201,21 +3212,21 @@
       <c r="F71" s="14"/>
       <c r="G71" s="15"/>
       <c r="H71" s="8" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J71" s="16" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C72" s="18"/>
       <c r="D72" s="18" t="s">
@@ -3227,18 +3238,18 @@
       <c r="F72" s="18"/>
       <c r="G72" s="19"/>
       <c r="H72" s="19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="I72" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J72" s="20" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A75" s="21" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.15">
@@ -3276,7 +3287,7 @@
       </c>
       <c r="G77" s="15"/>
       <c r="H77" s="15" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="I77" s="15"/>
       <c r="J77" s="16"/>
@@ -3318,13 +3329,13 @@
       <c r="F79" s="14"/>
       <c r="G79" s="15"/>
       <c r="H79" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="I79" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J79" s="16" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.15">
@@ -3348,7 +3359,7 @@
       <c r="H80" s="15"/>
       <c r="I80" s="15"/>
       <c r="J80" s="16" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.15">
@@ -3368,13 +3379,13 @@
       <c r="F81" s="14"/>
       <c r="G81" s="15"/>
       <c r="H81" s="15" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I81" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.15">
@@ -3393,10 +3404,10 @@
       <c r="G82" s="15"/>
       <c r="H82" s="15"/>
       <c r="I82" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J82" s="16" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.15">
@@ -3434,21 +3445,21 @@
       <c r="F84" s="14"/>
       <c r="G84" s="15"/>
       <c r="H84" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="I84" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J84" s="16" t="s">
         <v>153</v>
-      </c>
-      <c r="I84" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="J84" s="16" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A85" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C85" s="14"/>
       <c r="D85" s="14" t="s">
@@ -3460,21 +3471,21 @@
       <c r="F85" s="14"/>
       <c r="G85" s="15"/>
       <c r="H85" s="15" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J85" s="16" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A86" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C86" s="14"/>
       <c r="D86" s="14" t="s">
@@ -3484,7 +3495,7 @@
         <v>7</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G86" s="15"/>
       <c r="H86" s="15"/>
@@ -3493,10 +3504,10 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A87" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C87" s="14"/>
       <c r="D87" s="14" t="s">
@@ -3508,21 +3519,21 @@
       <c r="F87" s="14"/>
       <c r="G87" s="15"/>
       <c r="H87" s="15" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J87" s="16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C88" s="18"/>
       <c r="D88" s="18" t="s">
@@ -3534,18 +3545,18 @@
       <c r="F88" s="18"/>
       <c r="G88" s="19"/>
       <c r="H88" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I88" s="19" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J88" s="20" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A90" s="21" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.15">
@@ -3583,7 +3594,7 @@
       </c>
       <c r="G92" s="15"/>
       <c r="H92" s="15" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I92" s="15"/>
       <c r="J92" s="16"/>
@@ -3626,10 +3637,10 @@
       <c r="G94" s="15"/>
       <c r="H94" s="15"/>
       <c r="I94" s="14" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J94" s="16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.15">
@@ -3652,10 +3663,10 @@
       <c r="G95" s="15"/>
       <c r="H95" s="15"/>
       <c r="I95" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J95" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="27" x14ac:dyDescent="0.15">
@@ -3668,10 +3679,10 @@
       <c r="G96" s="15"/>
       <c r="H96" s="15"/>
       <c r="I96" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J96" s="16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.15">
@@ -3691,13 +3702,13 @@
       <c r="F97" s="14"/>
       <c r="G97" s="15"/>
       <c r="H97" s="15" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I97" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J97" s="16" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.15">
@@ -3716,10 +3727,10 @@
       <c r="G98" s="15"/>
       <c r="H98" s="15"/>
       <c r="I98" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J98" s="16" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.15">
@@ -3757,21 +3768,21 @@
       <c r="F100" s="14"/>
       <c r="G100" s="15"/>
       <c r="H100" s="15" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="I100" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J100" s="16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A101" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C101" s="14"/>
       <c r="D101" s="14" t="s">
@@ -3783,21 +3794,21 @@
       <c r="F101" s="14"/>
       <c r="G101" s="15"/>
       <c r="H101" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I101" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J101" s="16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A102" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C102" s="14"/>
       <c r="D102" s="14" t="s">
@@ -3807,25 +3818,25 @@
         <v>7</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G102" s="15"/>
       <c r="H102" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J102" s="16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A103" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C103" s="14"/>
       <c r="D103" s="14" t="s">
@@ -3837,21 +3848,21 @@
       <c r="F103" s="14"/>
       <c r="G103" s="15"/>
       <c r="H103" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J103" s="16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C104" s="18"/>
       <c r="D104" s="18" t="s">
@@ -3863,18 +3874,18 @@
       <c r="F104" s="18"/>
       <c r="G104" s="19"/>
       <c r="H104" s="19" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I104" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J104" s="20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A106" s="21" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.15">
@@ -3912,7 +3923,7 @@
       </c>
       <c r="G108" s="15"/>
       <c r="H108" s="15" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="I108" s="15"/>
       <c r="J108" s="16"/>
@@ -3954,13 +3965,13 @@
       <c r="F110" s="14"/>
       <c r="G110" s="15"/>
       <c r="H110" s="15" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="I110" s="14" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="J110" s="16" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.15">
@@ -3984,7 +3995,7 @@
       <c r="H111" s="15"/>
       <c r="I111" s="15"/>
       <c r="J111" s="16" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.15">
@@ -4004,13 +4015,13 @@
       <c r="F112" s="14"/>
       <c r="G112" s="15"/>
       <c r="H112" s="15" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I112" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J112" s="16" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.15">
@@ -4029,10 +4040,10 @@
       <c r="G113" s="15"/>
       <c r="H113" s="15"/>
       <c r="I113" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J113" s="16" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.15">
@@ -4070,21 +4081,21 @@
       <c r="F115" s="14"/>
       <c r="G115" s="15"/>
       <c r="H115" s="15" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="I115" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J115" s="16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A116" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C116" s="14"/>
       <c r="D116" s="14" t="s">
@@ -4096,21 +4107,21 @@
       <c r="F116" s="14"/>
       <c r="G116" s="15"/>
       <c r="H116" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J116" s="16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A117" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C117" s="14"/>
       <c r="D117" s="14" t="s">
@@ -4120,25 +4131,25 @@
         <v>7</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G117" s="15"/>
       <c r="H117" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J117" s="16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A118" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C118" s="14"/>
       <c r="D118" s="14" t="s">
@@ -4150,21 +4161,21 @@
       <c r="F118" s="14"/>
       <c r="G118" s="15"/>
       <c r="H118" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I118" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J118" s="16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C119" s="18"/>
       <c r="D119" s="18" t="s">
@@ -4176,18 +4187,18 @@
       <c r="F119" s="18"/>
       <c r="G119" s="19"/>
       <c r="H119" s="19" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I119" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J119" s="20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A121" s="21" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.15">
@@ -4225,7 +4236,7 @@
       </c>
       <c r="G123" s="15"/>
       <c r="H123" s="15" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="I123" s="15"/>
       <c r="J123" s="16"/>
@@ -4267,13 +4278,13 @@
       <c r="F125" s="14"/>
       <c r="G125" s="15"/>
       <c r="H125" s="15" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="I125" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J125" s="16" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.15">
@@ -4297,7 +4308,7 @@
       <c r="H126" s="15"/>
       <c r="I126" s="15"/>
       <c r="J126" s="16" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.15">
@@ -4317,13 +4328,13 @@
       <c r="F127" s="14"/>
       <c r="G127" s="15"/>
       <c r="H127" s="15" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I127" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J127" s="16" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.15">
@@ -4342,10 +4353,10 @@
       <c r="G128" s="15"/>
       <c r="H128" s="15"/>
       <c r="I128" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J128" s="16" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.15">
@@ -4383,21 +4394,21 @@
       <c r="F130" s="14"/>
       <c r="G130" s="15"/>
       <c r="H130" s="15" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="I130" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J130" s="16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A131" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C131" s="14"/>
       <c r="D131" s="14" t="s">
@@ -4409,21 +4420,21 @@
       <c r="F131" s="14"/>
       <c r="G131" s="15"/>
       <c r="H131" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I131" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J131" s="16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A132" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C132" s="14"/>
       <c r="D132" s="14" t="s">
@@ -4433,25 +4444,25 @@
         <v>7</v>
       </c>
       <c r="F132" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G132" s="15"/>
       <c r="H132" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I132" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J132" s="16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A133" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C133" s="14"/>
       <c r="D133" s="14" t="s">
@@ -4463,21 +4474,21 @@
       <c r="F133" s="14"/>
       <c r="G133" s="15"/>
       <c r="H133" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I133" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J133" s="16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="134" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B134" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C134" s="18"/>
       <c r="D134" s="18" t="s">
@@ -4489,18 +4500,18 @@
       <c r="F134" s="18"/>
       <c r="G134" s="19"/>
       <c r="H134" s="19" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I134" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J134" s="20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="136" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A136" s="21" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.15">
@@ -4538,7 +4549,7 @@
       </c>
       <c r="G138" s="15"/>
       <c r="H138" s="15" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="I138" s="15"/>
       <c r="J138" s="16"/>
@@ -4580,13 +4591,13 @@
       <c r="F140" s="14"/>
       <c r="G140" s="15"/>
       <c r="H140" s="15" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I140" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J140" s="16" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.15">
@@ -4610,7 +4621,7 @@
       <c r="H141" s="15"/>
       <c r="I141" s="15"/>
       <c r="J141" s="16" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.15">
@@ -4630,13 +4641,13 @@
       <c r="F142" s="14"/>
       <c r="G142" s="15"/>
       <c r="H142" s="15" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I142" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J142" s="16" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.15">
@@ -4655,10 +4666,10 @@
       <c r="G143" s="15"/>
       <c r="H143" s="15"/>
       <c r="I143" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J143" s="16" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.15">
@@ -4696,21 +4707,21 @@
       <c r="F145" s="14"/>
       <c r="G145" s="15"/>
       <c r="H145" s="15" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="I145" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J145" s="16" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A146" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C146" s="14"/>
       <c r="D146" s="14" t="s">
@@ -4722,21 +4733,21 @@
       <c r="F146" s="14"/>
       <c r="G146" s="15"/>
       <c r="H146" s="15" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I146" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J146" s="16" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A147" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B147" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C147" s="14"/>
       <c r="D147" s="14" t="s">
@@ -4746,25 +4757,25 @@
         <v>7</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G147" s="15"/>
       <c r="H147" s="8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="I147" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J147" s="16" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A148" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C148" s="14"/>
       <c r="D148" s="14" t="s">
@@ -4781,10 +4792,10 @@
     </row>
     <row r="149" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B149" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C149" s="18"/>
       <c r="D149" s="18" t="s">
@@ -4796,18 +4807,18 @@
       <c r="F149" s="18"/>
       <c r="G149" s="19"/>
       <c r="H149" s="19" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="I149" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J149" s="20" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="151" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A151" s="21" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.15">
@@ -4845,7 +4856,7 @@
       </c>
       <c r="G153" s="15"/>
       <c r="H153" s="15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="I153" s="15"/>
       <c r="J153" s="16"/>
@@ -4887,13 +4898,13 @@
       <c r="F155" s="14"/>
       <c r="G155" s="15"/>
       <c r="H155" s="15" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="I155" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J155" s="16" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.15">
@@ -4917,7 +4928,7 @@
       <c r="H156" s="15"/>
       <c r="I156" s="15"/>
       <c r="J156" s="16" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.15">
@@ -4937,13 +4948,13 @@
       <c r="F157" s="14"/>
       <c r="G157" s="15"/>
       <c r="H157" s="15" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I157" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J157" s="16" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.15">
@@ -4962,10 +4973,10 @@
       <c r="G158" s="15"/>
       <c r="H158" s="15"/>
       <c r="I158" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J158" s="16" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.15">
@@ -5003,21 +5014,21 @@
       <c r="F160" s="14"/>
       <c r="G160" s="15"/>
       <c r="H160" s="15" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="I160" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J160" s="16" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A161" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C161" s="14"/>
       <c r="D161" s="14" t="s">
@@ -5029,21 +5040,21 @@
       <c r="F161" s="14"/>
       <c r="G161" s="15"/>
       <c r="H161" s="15" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I161" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J161" s="16" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A162" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C162" s="14"/>
       <c r="D162" s="14" t="s">
@@ -5053,25 +5064,25 @@
         <v>7</v>
       </c>
       <c r="F162" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G162" s="15"/>
       <c r="H162" s="8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="I162" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J162" s="16" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A163" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C163" s="14"/>
       <c r="D163" s="14" t="s">
@@ -5088,10 +5099,10 @@
     </row>
     <row r="164" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B164" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C164" s="18"/>
       <c r="D164" s="18" t="s">
@@ -5103,18 +5114,18 @@
       <c r="F164" s="18"/>
       <c r="G164" s="19"/>
       <c r="H164" s="19" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="I164" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J164" s="20" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A166" s="21" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.15">
@@ -5152,7 +5163,7 @@
       </c>
       <c r="G168" s="15"/>
       <c r="H168" s="15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="I168" s="15"/>
       <c r="J168" s="16"/>
@@ -5194,13 +5205,13 @@
       <c r="F170" s="14"/>
       <c r="G170" s="15"/>
       <c r="H170" s="15" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="I170" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J170" s="16" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.15">
@@ -5224,7 +5235,7 @@
       <c r="H171" s="15"/>
       <c r="I171" s="15"/>
       <c r="J171" s="16" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.15">
@@ -5244,13 +5255,13 @@
       <c r="F172" s="14"/>
       <c r="G172" s="15"/>
       <c r="H172" s="15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="I172" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J172" s="16" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.15">
@@ -5269,10 +5280,10 @@
       <c r="G173" s="15"/>
       <c r="H173" s="15"/>
       <c r="I173" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J173" s="16" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.15">
@@ -5310,21 +5321,21 @@
       <c r="F175" s="14"/>
       <c r="G175" s="15"/>
       <c r="H175" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I175" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J175" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A176" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C176" s="14"/>
       <c r="D176" s="14" t="s">
@@ -5336,21 +5347,21 @@
       <c r="F176" s="14"/>
       <c r="G176" s="15"/>
       <c r="H176" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I176" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J176" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A177" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C177" s="14"/>
       <c r="D177" s="14" t="s">
@@ -5360,7 +5371,7 @@
         <v>7</v>
       </c>
       <c r="F177" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G177" s="15"/>
       <c r="H177" s="8"/>
@@ -5369,10 +5380,10 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A178" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C178" s="14"/>
       <c r="D178" s="14" t="s">
@@ -5384,21 +5395,21 @@
       <c r="F178" s="14"/>
       <c r="G178" s="15"/>
       <c r="H178" s="8" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="I178" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J178" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="179" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B179" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C179" s="18"/>
       <c r="D179" s="18" t="s">
@@ -5410,18 +5421,18 @@
       <c r="F179" s="18"/>
       <c r="G179" s="19"/>
       <c r="H179" s="19" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="I179" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J179" s="20" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="181" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A181" s="21" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.15">
@@ -5459,7 +5470,7 @@
       </c>
       <c r="G183" s="15"/>
       <c r="H183" s="15" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="I183" s="15"/>
       <c r="J183" s="16"/>
@@ -5501,13 +5512,13 @@
       <c r="F185" s="14"/>
       <c r="G185" s="15"/>
       <c r="H185" s="15" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="I185" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J185" s="16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.15">
@@ -5531,7 +5542,7 @@
       <c r="H186" s="15"/>
       <c r="I186" s="15"/>
       <c r="J186" s="16" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.15">
@@ -5551,13 +5562,13 @@
       <c r="F187" s="14"/>
       <c r="G187" s="15"/>
       <c r="H187" s="15" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I187" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J187" s="16" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.15">
@@ -5576,10 +5587,10 @@
       <c r="G188" s="15"/>
       <c r="H188" s="15"/>
       <c r="I188" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J188" s="16" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.15">
@@ -5622,10 +5633,10 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A191" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C191" s="14"/>
       <c r="D191" s="14" t="s">
@@ -5642,10 +5653,10 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A192" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C192" s="14"/>
       <c r="D192" s="14" t="s">
@@ -5655,7 +5666,7 @@
         <v>7</v>
       </c>
       <c r="F192" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G192" s="15"/>
       <c r="H192" s="8"/>
@@ -5664,10 +5675,10 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A193" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C193" s="14"/>
       <c r="D193" s="14" t="s">
@@ -5684,10 +5695,10 @@
     </row>
     <row r="194" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B194" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C194" s="18"/>
       <c r="D194" s="18" t="s">
@@ -5699,18 +5710,18 @@
       <c r="F194" s="18"/>
       <c r="G194" s="19"/>
       <c r="H194" s="19" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I194" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J194" s="20" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="196" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A196" s="21" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.15">
@@ -5748,13 +5759,13 @@
       </c>
       <c r="G198" s="15"/>
       <c r="H198" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I198" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J198" s="16" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.15">
@@ -5774,13 +5785,13 @@
       <c r="F199" s="14"/>
       <c r="G199" s="15"/>
       <c r="H199" s="15" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I199" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J199" s="16" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.15">
@@ -5800,13 +5811,13 @@
       <c r="F200" s="14"/>
       <c r="G200" s="15"/>
       <c r="H200" s="15" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I200" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J200" s="16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.15">
@@ -5830,7 +5841,7 @@
       <c r="H201" s="15"/>
       <c r="I201" s="15"/>
       <c r="J201" s="16" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.15">
@@ -5850,13 +5861,13 @@
       <c r="F202" s="14"/>
       <c r="G202" s="15"/>
       <c r="H202" s="15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="I202" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J202" s="16" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.15">
@@ -5875,10 +5886,10 @@
       <c r="G203" s="15"/>
       <c r="H203" s="15"/>
       <c r="I203" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J203" s="16" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.15">
@@ -5916,21 +5927,21 @@
       <c r="F205" s="14"/>
       <c r="G205" s="15"/>
       <c r="H205" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I205" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J205" s="16" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A206" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B206" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C206" s="14"/>
       <c r="D206" s="14" t="s">
@@ -5942,21 +5953,21 @@
       <c r="F206" s="14"/>
       <c r="G206" s="15"/>
       <c r="H206" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I206" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J206" s="16" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A207" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B207" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C207" s="14"/>
       <c r="D207" s="14" t="s">
@@ -5966,7 +5977,7 @@
         <v>7</v>
       </c>
       <c r="F207" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G207" s="15"/>
       <c r="H207" s="8"/>
@@ -5975,10 +5986,10 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A208" s="22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B208" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C208" s="14"/>
       <c r="D208" s="14" t="s">
@@ -5990,21 +6001,21 @@
       <c r="F208" s="14"/>
       <c r="G208" s="15"/>
       <c r="H208" s="8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="I208" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J208" s="16" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="209" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A209" s="17" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B209" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C209" s="18"/>
       <c r="D209" s="18" t="s">
@@ -6016,13 +6027,13 @@
       <c r="F209" s="18"/>
       <c r="G209" s="19"/>
       <c r="H209" s="19" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I209" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J209" s="20" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>